<commit_message>
updated balde and producao
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2025-11.xlsx
+++ b/first-atlas/producao_2025-11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29525"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86D7484-B4D8-4E59-8925-92E33A071C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3169D299-4022-4B23-8954-7BC7065F35A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{3FA0812B-7F53-402D-BAE5-61E81C02CB4E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{3FA0812B-7F53-402D-BAE5-61E81C02CB4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7686" uniqueCount="3128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7704" uniqueCount="3134">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -8156,15 +8156,9 @@
     <t>CONSULTEXTIL CONSULTORIA LTDA</t>
   </si>
   <si>
-    <t xml:space="preserve">Ata de eleicao da diretoria com mandato vigente, devidamente registrado no orgao competente.&lt;br&gt;&lt;br&gt;Estatuto social atualizado e registrado no orgao competente	</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estatuto social atualizado e registrado no orgao competente&lt;br&gt;&lt;br&gt;Ata de eleicao da diretoria  com mandato vigente, devidamente registrado no orgao competente </t>
   </si>
   <si>
-    <t xml:space="preserve">Contrato social da empresa VOOX ENGENHARIA LTDA, atualizado e registrado no orgao competente, com a devida clausula de administracao. </t>
-  </si>
-  <si>
     <t>61307587000170</t>
   </si>
   <si>
@@ -9423,6 +9417,30 @@
   </si>
   <si>
     <t>PAULO HENRIQUE GONZAGA SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>53363466000118</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LEONARDO TORRES DE SOUSA</t>
+  </si>
+  <si>
+    <t>62660713000139</t>
+  </si>
+  <si>
+    <t>LF CONSULTORIA E ADMINISTRACOES LTDA</t>
+  </si>
+  <si>
+    <t>63504262000103</t>
+  </si>
+  <si>
+    <t>F F DA SIVA</t>
+  </si>
+  <si>
+    <t>38798871000175</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ANTONIO JOSE OLIVEIRA DA SILVA FORTES</t>
   </si>
 </sst>
 </file>
@@ -9794,9 +9812,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCD3CE2-DBA2-4F4F-B6A3-11EE884EA727}">
-  <dimension ref="A1:G1529"/>
+  <dimension ref="A1:G1533"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1507" workbookViewId="0">
+      <selection activeCell="A1532" sqref="A1532"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9919,7 +9939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45964</v>
       </c>
@@ -10996,8 +11016,8 @@
       <c r="F52" t="s">
         <v>28</v>
       </c>
-      <c r="G52">
-        <v>0</v>
+      <c r="G52" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -11939,6 +11959,9 @@
       <c r="F93" t="s">
         <v>28</v>
       </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
@@ -15708,8 +15731,8 @@
       <c r="F257" t="s">
         <v>101</v>
       </c>
-      <c r="G257" t="s">
-        <v>2705</v>
+      <c r="G257" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
@@ -20722,8 +20745,8 @@
       <c r="F475" t="s">
         <v>23</v>
       </c>
-      <c r="G475">
-        <v>0</v>
+      <c r="G475" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="476" spans="1:7" x14ac:dyDescent="0.25">
@@ -25575,8 +25598,8 @@
       <c r="F686" t="s">
         <v>28</v>
       </c>
-      <c r="G686">
-        <v>0</v>
+      <c r="G686" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="687" spans="1:7" x14ac:dyDescent="0.25">
@@ -25621,6 +25644,9 @@
       <c r="F688" t="s">
         <v>28</v>
       </c>
+      <c r="G688">
+        <v>0</v>
+      </c>
     </row>
     <row r="689" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A689" s="1">
@@ -26559,10 +26585,10 @@
         <v>9</v>
       </c>
       <c r="F729" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="G729" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
     </row>
     <row r="730" spans="1:7" x14ac:dyDescent="0.25">
@@ -30104,7 +30130,7 @@
         <v>101</v>
       </c>
       <c r="G883" t="s">
-        <v>3013</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="884" spans="1:7" x14ac:dyDescent="0.25">
@@ -36035,7 +36061,7 @@
         <v>9</v>
       </c>
       <c r="F1141" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G1141">
         <v>0</v>
@@ -36219,7 +36245,7 @@
         <v>9</v>
       </c>
       <c r="F1149" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G1149">
         <v>0</v>
@@ -37001,7 +37027,7 @@
         <v>9</v>
       </c>
       <c r="F1183" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="G1183" t="s">
         <v>2538</v>
@@ -37461,7 +37487,7 @@
         <v>27</v>
       </c>
       <c r="F1203" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G1203">
         <v>0</v>
@@ -38105,10 +38131,10 @@
         <v>730</v>
       </c>
       <c r="F1231" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1231" t="s">
-        <v>2707</v>
+        <v>28</v>
+      </c>
+      <c r="G1231">
+        <v>0</v>
       </c>
     </row>
     <row r="1232" spans="1:7" x14ac:dyDescent="0.25">
@@ -38128,7 +38154,7 @@
         <v>9</v>
       </c>
       <c r="F1232" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G1232">
         <v>0</v>
@@ -38208,10 +38234,10 @@
         <v>45983</v>
       </c>
       <c r="B1236" t="s">
-        <v>2708</v>
+        <v>2706</v>
       </c>
       <c r="C1236" t="s">
-        <v>2709</v>
+        <v>2707</v>
       </c>
       <c r="D1236" t="s">
         <v>74</v>
@@ -38404,7 +38430,7 @@
         <v>27</v>
       </c>
       <c r="F1244" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="G1244" t="s">
         <v>2538</v>
@@ -39925,7 +39951,7 @@
         <v>101</v>
       </c>
       <c r="G1310" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="1311" spans="1:7" x14ac:dyDescent="0.25">
@@ -40071,10 +40097,10 @@
         <v>45986</v>
       </c>
       <c r="B1317" t="s">
-        <v>2710</v>
+        <v>2708</v>
       </c>
       <c r="C1317" t="s">
-        <v>2711</v>
+        <v>2709</v>
       </c>
       <c r="D1317" t="s">
         <v>424</v>
@@ -40094,10 +40120,10 @@
         <v>45986</v>
       </c>
       <c r="B1318" t="s">
-        <v>2712</v>
+        <v>2710</v>
       </c>
       <c r="C1318" t="s">
-        <v>2713</v>
+        <v>2711</v>
       </c>
       <c r="D1318" t="s">
         <v>424</v>
@@ -40117,10 +40143,10 @@
         <v>45986</v>
       </c>
       <c r="B1319" t="s">
-        <v>2714</v>
+        <v>2712</v>
       </c>
       <c r="C1319" t="s">
-        <v>2715</v>
+        <v>2713</v>
       </c>
       <c r="D1319" t="s">
         <v>424</v>
@@ -40140,10 +40166,10 @@
         <v>45986</v>
       </c>
       <c r="B1320" t="s">
-        <v>2716</v>
+        <v>2714</v>
       </c>
       <c r="C1320" t="s">
-        <v>2717</v>
+        <v>2715</v>
       </c>
       <c r="D1320" t="s">
         <v>424</v>
@@ -40163,10 +40189,10 @@
         <v>45986</v>
       </c>
       <c r="B1321" t="s">
-        <v>2718</v>
+        <v>2716</v>
       </c>
       <c r="C1321" t="s">
-        <v>2719</v>
+        <v>2717</v>
       </c>
       <c r="D1321" t="s">
         <v>424</v>
@@ -40186,10 +40212,10 @@
         <v>45986</v>
       </c>
       <c r="B1322" t="s">
-        <v>2720</v>
+        <v>2718</v>
       </c>
       <c r="C1322" t="s">
-        <v>2721</v>
+        <v>2719</v>
       </c>
       <c r="D1322" t="s">
         <v>424</v>
@@ -40209,10 +40235,10 @@
         <v>45986</v>
       </c>
       <c r="B1323" t="s">
-        <v>2722</v>
+        <v>2720</v>
       </c>
       <c r="C1323" t="s">
-        <v>2723</v>
+        <v>2721</v>
       </c>
       <c r="D1323" t="s">
         <v>424</v>
@@ -40232,10 +40258,10 @@
         <v>45986</v>
       </c>
       <c r="B1324" t="s">
-        <v>2724</v>
+        <v>2722</v>
       </c>
       <c r="C1324" t="s">
-        <v>2725</v>
+        <v>2723</v>
       </c>
       <c r="D1324" t="s">
         <v>424</v>
@@ -40255,10 +40281,10 @@
         <v>45986</v>
       </c>
       <c r="B1325" t="s">
-        <v>2726</v>
+        <v>2724</v>
       </c>
       <c r="C1325" t="s">
-        <v>2727</v>
+        <v>2725</v>
       </c>
       <c r="D1325" t="s">
         <v>424</v>
@@ -40278,10 +40304,10 @@
         <v>45986</v>
       </c>
       <c r="B1326" t="s">
-        <v>2728</v>
+        <v>2726</v>
       </c>
       <c r="C1326" t="s">
-        <v>2729</v>
+        <v>2727</v>
       </c>
       <c r="D1326" t="s">
         <v>39</v>
@@ -40301,10 +40327,10 @@
         <v>45986</v>
       </c>
       <c r="B1327" t="s">
-        <v>2730</v>
+        <v>2728</v>
       </c>
       <c r="C1327" t="s">
-        <v>2731</v>
+        <v>2729</v>
       </c>
       <c r="D1327" t="s">
         <v>13</v>
@@ -40324,10 +40350,10 @@
         <v>45986</v>
       </c>
       <c r="B1328" t="s">
-        <v>2732</v>
+        <v>2730</v>
       </c>
       <c r="C1328" t="s">
-        <v>2733</v>
+        <v>2731</v>
       </c>
       <c r="D1328" t="s">
         <v>26</v>
@@ -40347,10 +40373,10 @@
         <v>45986</v>
       </c>
       <c r="B1329" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C1329" t="s">
-        <v>2735</v>
+        <v>2733</v>
       </c>
       <c r="D1329" t="s">
         <v>50</v>
@@ -40370,10 +40396,10 @@
         <v>45986</v>
       </c>
       <c r="B1330" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="C1330" t="s">
-        <v>2737</v>
+        <v>2735</v>
       </c>
       <c r="D1330" t="s">
         <v>39</v>
@@ -40393,10 +40419,10 @@
         <v>45986</v>
       </c>
       <c r="B1331" t="s">
-        <v>2738</v>
+        <v>2736</v>
       </c>
       <c r="C1331" t="s">
-        <v>2739</v>
+        <v>2737</v>
       </c>
       <c r="D1331" t="s">
         <v>34</v>
@@ -40416,10 +40442,10 @@
         <v>45986</v>
       </c>
       <c r="B1332" t="s">
-        <v>2740</v>
+        <v>2738</v>
       </c>
       <c r="C1332" t="s">
-        <v>2741</v>
+        <v>2739</v>
       </c>
       <c r="D1332" t="s">
         <v>74</v>
@@ -40439,10 +40465,10 @@
         <v>45986</v>
       </c>
       <c r="B1333" t="s">
-        <v>2742</v>
+        <v>2740</v>
       </c>
       <c r="C1333" t="s">
-        <v>2743</v>
+        <v>2741</v>
       </c>
       <c r="D1333" t="s">
         <v>26</v>
@@ -40462,10 +40488,10 @@
         <v>45986</v>
       </c>
       <c r="B1334" t="s">
-        <v>2744</v>
+        <v>2742</v>
       </c>
       <c r="C1334" t="s">
-        <v>2745</v>
+        <v>2743</v>
       </c>
       <c r="D1334" t="s">
         <v>74</v>
@@ -40485,10 +40511,10 @@
         <v>45986</v>
       </c>
       <c r="B1335" t="s">
-        <v>2746</v>
+        <v>2744</v>
       </c>
       <c r="C1335" t="s">
-        <v>2747</v>
+        <v>2745</v>
       </c>
       <c r="D1335" t="s">
         <v>39</v>
@@ -40508,10 +40534,10 @@
         <v>45986</v>
       </c>
       <c r="B1336" t="s">
-        <v>2748</v>
+        <v>2746</v>
       </c>
       <c r="C1336" t="s">
-        <v>2749</v>
+        <v>2747</v>
       </c>
       <c r="D1336" t="s">
         <v>59</v>
@@ -40531,10 +40557,10 @@
         <v>45986</v>
       </c>
       <c r="B1337" t="s">
-        <v>2750</v>
+        <v>2748</v>
       </c>
       <c r="C1337" t="s">
-        <v>2751</v>
+        <v>2749</v>
       </c>
       <c r="D1337" t="s">
         <v>34</v>
@@ -40554,10 +40580,10 @@
         <v>45986</v>
       </c>
       <c r="B1338" t="s">
-        <v>2752</v>
+        <v>2750</v>
       </c>
       <c r="C1338" t="s">
-        <v>2753</v>
+        <v>2751</v>
       </c>
       <c r="D1338" t="s">
         <v>13</v>
@@ -40577,10 +40603,10 @@
         <v>45986</v>
       </c>
       <c r="B1339" t="s">
-        <v>2754</v>
+        <v>2752</v>
       </c>
       <c r="C1339" t="s">
-        <v>2755</v>
+        <v>2753</v>
       </c>
       <c r="D1339" t="s">
         <v>31</v>
@@ -40600,10 +40626,10 @@
         <v>45986</v>
       </c>
       <c r="B1340" t="s">
-        <v>2756</v>
+        <v>2754</v>
       </c>
       <c r="C1340" t="s">
-        <v>2757</v>
+        <v>2755</v>
       </c>
       <c r="D1340" t="s">
         <v>50</v>
@@ -40623,7 +40649,7 @@
         <v>45986</v>
       </c>
       <c r="B1341" t="s">
-        <v>2758</v>
+        <v>2756</v>
       </c>
       <c r="D1341" t="s">
         <v>21</v>
@@ -40643,10 +40669,10 @@
         <v>45986</v>
       </c>
       <c r="B1342" t="s">
-        <v>2759</v>
+        <v>2757</v>
       </c>
       <c r="C1342" t="s">
-        <v>2760</v>
+        <v>2758</v>
       </c>
       <c r="D1342" t="s">
         <v>44</v>
@@ -40666,10 +40692,10 @@
         <v>45986</v>
       </c>
       <c r="B1343" t="s">
-        <v>2761</v>
+        <v>2759</v>
       </c>
       <c r="C1343" t="s">
-        <v>2762</v>
+        <v>2760</v>
       </c>
       <c r="D1343" t="s">
         <v>644</v>
@@ -40689,10 +40715,10 @@
         <v>45986</v>
       </c>
       <c r="B1344" t="s">
-        <v>2763</v>
+        <v>2761</v>
       </c>
       <c r="C1344" t="s">
-        <v>2764</v>
+        <v>2762</v>
       </c>
       <c r="D1344" t="s">
         <v>59</v>
@@ -40712,10 +40738,10 @@
         <v>45986</v>
       </c>
       <c r="B1345" t="s">
-        <v>2765</v>
+        <v>2763</v>
       </c>
       <c r="C1345" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="D1345" t="s">
         <v>17</v>
@@ -40758,10 +40784,10 @@
         <v>45986</v>
       </c>
       <c r="B1347" t="s">
-        <v>2767</v>
+        <v>2765</v>
       </c>
       <c r="C1347" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="D1347" t="s">
         <v>31</v>
@@ -40781,10 +40807,10 @@
         <v>45986</v>
       </c>
       <c r="B1348" t="s">
-        <v>2769</v>
+        <v>2767</v>
       </c>
       <c r="C1348" t="s">
-        <v>2770</v>
+        <v>2768</v>
       </c>
       <c r="D1348" t="s">
         <v>8</v>
@@ -40804,10 +40830,10 @@
         <v>45986</v>
       </c>
       <c r="B1349" t="s">
-        <v>2771</v>
+        <v>2769</v>
       </c>
       <c r="C1349" t="s">
-        <v>2772</v>
+        <v>2770</v>
       </c>
       <c r="D1349" t="s">
         <v>47</v>
@@ -40827,10 +40853,10 @@
         <v>45986</v>
       </c>
       <c r="B1350" t="s">
-        <v>2773</v>
+        <v>2771</v>
       </c>
       <c r="C1350" t="s">
-        <v>2774</v>
+        <v>2772</v>
       </c>
       <c r="D1350" t="s">
         <v>59</v>
@@ -40842,7 +40868,7 @@
         <v>14</v>
       </c>
       <c r="G1350" t="s">
-        <v>3014</v>
+        <v>3012</v>
       </c>
     </row>
     <row r="1351" spans="1:7" x14ac:dyDescent="0.25">
@@ -40850,10 +40876,10 @@
         <v>45986</v>
       </c>
       <c r="B1351" t="s">
-        <v>2775</v>
+        <v>2773</v>
       </c>
       <c r="C1351" t="s">
-        <v>2776</v>
+        <v>2774</v>
       </c>
       <c r="D1351" t="s">
         <v>59</v>
@@ -40873,10 +40899,10 @@
         <v>45986</v>
       </c>
       <c r="B1352" t="s">
-        <v>2777</v>
+        <v>2775</v>
       </c>
       <c r="C1352" t="s">
-        <v>2778</v>
+        <v>2776</v>
       </c>
       <c r="D1352" t="s">
         <v>44</v>
@@ -40896,10 +40922,10 @@
         <v>45986</v>
       </c>
       <c r="B1353" t="s">
-        <v>2779</v>
+        <v>2777</v>
       </c>
       <c r="C1353" t="s">
-        <v>2780</v>
+        <v>2778</v>
       </c>
       <c r="D1353" t="s">
         <v>59</v>
@@ -40919,10 +40945,10 @@
         <v>45986</v>
       </c>
       <c r="B1354" t="s">
-        <v>2781</v>
+        <v>2779</v>
       </c>
       <c r="C1354" t="s">
-        <v>2782</v>
+        <v>2780</v>
       </c>
       <c r="D1354" t="s">
         <v>59</v>
@@ -40942,10 +40968,10 @@
         <v>45986</v>
       </c>
       <c r="B1355" t="s">
-        <v>2783</v>
+        <v>2781</v>
       </c>
       <c r="C1355" t="s">
-        <v>2784</v>
+        <v>2782</v>
       </c>
       <c r="D1355" t="s">
         <v>44</v>
@@ -40965,10 +40991,10 @@
         <v>45986</v>
       </c>
       <c r="B1356" t="s">
-        <v>2785</v>
+        <v>2783</v>
       </c>
       <c r="C1356" t="s">
-        <v>2786</v>
+        <v>2784</v>
       </c>
       <c r="D1356" t="s">
         <v>34</v>
@@ -40988,10 +41014,10 @@
         <v>45986</v>
       </c>
       <c r="B1357" t="s">
-        <v>2787</v>
+        <v>2785</v>
       </c>
       <c r="C1357" t="s">
-        <v>2788</v>
+        <v>2786</v>
       </c>
       <c r="D1357" t="s">
         <v>47</v>
@@ -41011,10 +41037,10 @@
         <v>45986</v>
       </c>
       <c r="B1358" t="s">
-        <v>2789</v>
+        <v>2787</v>
       </c>
       <c r="C1358" t="s">
-        <v>2790</v>
+        <v>2788</v>
       </c>
       <c r="D1358" t="s">
         <v>17</v>
@@ -41034,10 +41060,10 @@
         <v>45986</v>
       </c>
       <c r="B1359" t="s">
-        <v>2791</v>
+        <v>2789</v>
       </c>
       <c r="C1359" t="s">
-        <v>2792</v>
+        <v>2790</v>
       </c>
       <c r="D1359" t="s">
         <v>44</v>
@@ -41080,10 +41106,10 @@
         <v>45986</v>
       </c>
       <c r="B1361" t="s">
-        <v>2793</v>
+        <v>2791</v>
       </c>
       <c r="C1361" t="s">
-        <v>2794</v>
+        <v>2792</v>
       </c>
       <c r="D1361" t="s">
         <v>31</v>
@@ -41103,10 +41129,10 @@
         <v>45986</v>
       </c>
       <c r="B1362" t="s">
-        <v>2795</v>
+        <v>2793</v>
       </c>
       <c r="C1362" t="s">
-        <v>2796</v>
+        <v>2794</v>
       </c>
       <c r="D1362" t="s">
         <v>31</v>
@@ -41126,10 +41152,10 @@
         <v>45986</v>
       </c>
       <c r="B1363" t="s">
-        <v>2797</v>
+        <v>2795</v>
       </c>
       <c r="C1363" t="s">
-        <v>2798</v>
+        <v>2796</v>
       </c>
       <c r="D1363" t="s">
         <v>8</v>
@@ -41149,10 +41175,10 @@
         <v>45986</v>
       </c>
       <c r="B1364" t="s">
-        <v>2799</v>
+        <v>2797</v>
       </c>
       <c r="C1364" t="s">
-        <v>2800</v>
+        <v>2798</v>
       </c>
       <c r="D1364" t="s">
         <v>31</v>
@@ -41172,10 +41198,10 @@
         <v>45986</v>
       </c>
       <c r="B1365" t="s">
-        <v>2801</v>
+        <v>2799</v>
       </c>
       <c r="C1365" t="s">
-        <v>2802</v>
+        <v>2800</v>
       </c>
       <c r="D1365" t="s">
         <v>74</v>
@@ -41195,10 +41221,10 @@
         <v>45986</v>
       </c>
       <c r="B1366" t="s">
-        <v>2803</v>
+        <v>2801</v>
       </c>
       <c r="C1366" t="s">
-        <v>2804</v>
+        <v>2802</v>
       </c>
       <c r="D1366" t="s">
         <v>50</v>
@@ -41218,10 +41244,10 @@
         <v>45986</v>
       </c>
       <c r="B1367" t="s">
-        <v>2805</v>
+        <v>2803</v>
       </c>
       <c r="C1367" t="s">
-        <v>2806</v>
+        <v>2804</v>
       </c>
       <c r="D1367" t="s">
         <v>155</v>
@@ -41241,10 +41267,10 @@
         <v>45986</v>
       </c>
       <c r="B1368" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="C1368" t="s">
-        <v>2808</v>
+        <v>2806</v>
       </c>
       <c r="D1368" t="s">
         <v>8</v>
@@ -41264,10 +41290,10 @@
         <v>45986</v>
       </c>
       <c r="B1369" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
       <c r="C1369" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="D1369" t="s">
         <v>17</v>
@@ -41287,10 +41313,10 @@
         <v>45986</v>
       </c>
       <c r="B1370" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
       <c r="C1370" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
       <c r="D1370" t="s">
         <v>155</v>
@@ -41310,10 +41336,10 @@
         <v>45986</v>
       </c>
       <c r="B1371" t="s">
-        <v>2813</v>
+        <v>2811</v>
       </c>
       <c r="C1371" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
       <c r="D1371" t="s">
         <v>47</v>
@@ -41333,10 +41359,10 @@
         <v>45986</v>
       </c>
       <c r="B1372" t="s">
-        <v>2815</v>
+        <v>2813</v>
       </c>
       <c r="C1372" t="s">
-        <v>2816</v>
+        <v>2814</v>
       </c>
       <c r="D1372" t="s">
         <v>644</v>
@@ -41356,10 +41382,10 @@
         <v>45986</v>
       </c>
       <c r="B1373" t="s">
-        <v>2817</v>
+        <v>2815</v>
       </c>
       <c r="C1373" t="s">
-        <v>2818</v>
+        <v>2816</v>
       </c>
       <c r="D1373" t="s">
         <v>26</v>
@@ -41379,10 +41405,10 @@
         <v>45986</v>
       </c>
       <c r="B1374" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
       <c r="C1374" t="s">
-        <v>2820</v>
+        <v>2818</v>
       </c>
       <c r="D1374" t="s">
         <v>17</v>
@@ -41402,10 +41428,10 @@
         <v>45986</v>
       </c>
       <c r="B1375" t="s">
-        <v>2821</v>
+        <v>2819</v>
       </c>
       <c r="C1375" t="s">
-        <v>2822</v>
+        <v>2820</v>
       </c>
       <c r="D1375" t="s">
         <v>13</v>
@@ -41425,10 +41451,10 @@
         <v>45986</v>
       </c>
       <c r="B1376" t="s">
-        <v>2823</v>
+        <v>2821</v>
       </c>
       <c r="C1376" t="s">
-        <v>2824</v>
+        <v>2822</v>
       </c>
       <c r="D1376" t="s">
         <v>44</v>
@@ -41448,10 +41474,10 @@
         <v>45986</v>
       </c>
       <c r="B1377" t="s">
-        <v>2825</v>
+        <v>2823</v>
       </c>
       <c r="C1377" t="s">
-        <v>2826</v>
+        <v>2824</v>
       </c>
       <c r="D1377" t="s">
         <v>74</v>
@@ -41471,10 +41497,10 @@
         <v>45986</v>
       </c>
       <c r="B1378" t="s">
-        <v>2827</v>
+        <v>2825</v>
       </c>
       <c r="C1378" t="s">
-        <v>2828</v>
+        <v>2826</v>
       </c>
       <c r="D1378" t="s">
         <v>26</v>
@@ -41494,10 +41520,10 @@
         <v>45986</v>
       </c>
       <c r="B1379" t="s">
-        <v>2829</v>
+        <v>2827</v>
       </c>
       <c r="C1379" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="D1379" t="s">
         <v>59</v>
@@ -41517,10 +41543,10 @@
         <v>45986</v>
       </c>
       <c r="B1380" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="C1380" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
       <c r="D1380" t="s">
         <v>44</v>
@@ -41540,10 +41566,10 @@
         <v>45986</v>
       </c>
       <c r="B1381" t="s">
-        <v>2833</v>
+        <v>2831</v>
       </c>
       <c r="C1381" t="s">
-        <v>2834</v>
+        <v>2832</v>
       </c>
       <c r="D1381" t="s">
         <v>59</v>
@@ -41563,10 +41589,10 @@
         <v>45986</v>
       </c>
       <c r="B1382" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="C1382" t="s">
-        <v>2836</v>
+        <v>2834</v>
       </c>
       <c r="D1382" t="s">
         <v>644</v>
@@ -41586,10 +41612,10 @@
         <v>45986</v>
       </c>
       <c r="B1383" t="s">
-        <v>2837</v>
+        <v>2835</v>
       </c>
       <c r="C1383" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="D1383" t="s">
         <v>50</v>
@@ -41609,10 +41635,10 @@
         <v>45986</v>
       </c>
       <c r="B1384" t="s">
-        <v>2839</v>
+        <v>2837</v>
       </c>
       <c r="C1384" t="s">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="D1384" t="s">
         <v>2205</v>
@@ -41655,10 +41681,10 @@
         <v>45986</v>
       </c>
       <c r="B1386" t="s">
-        <v>2841</v>
+        <v>2839</v>
       </c>
       <c r="C1386" t="s">
-        <v>2842</v>
+        <v>2840</v>
       </c>
       <c r="D1386" t="s">
         <v>59</v>
@@ -41678,10 +41704,10 @@
         <v>45986</v>
       </c>
       <c r="B1387" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="C1387" t="s">
-        <v>2844</v>
+        <v>2842</v>
       </c>
       <c r="D1387" t="s">
         <v>34</v>
@@ -41701,10 +41727,10 @@
         <v>45986</v>
       </c>
       <c r="B1388" t="s">
-        <v>2845</v>
+        <v>2843</v>
       </c>
       <c r="C1388" t="s">
-        <v>2846</v>
+        <v>2844</v>
       </c>
       <c r="D1388" t="s">
         <v>8</v>
@@ -41724,10 +41750,10 @@
         <v>45986</v>
       </c>
       <c r="B1389" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="C1389" t="s">
-        <v>2848</v>
+        <v>2846</v>
       </c>
       <c r="D1389" t="s">
         <v>31</v>
@@ -41747,10 +41773,10 @@
         <v>45986</v>
       </c>
       <c r="B1390" t="s">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="C1390" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="D1390" t="s">
         <v>59</v>
@@ -41770,10 +41796,10 @@
         <v>45987</v>
       </c>
       <c r="B1391" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="C1391" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="D1391" t="s">
         <v>26</v>
@@ -41793,10 +41819,10 @@
         <v>45987</v>
       </c>
       <c r="B1392" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="C1392" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="D1392" t="s">
         <v>224</v>
@@ -41816,10 +41842,10 @@
         <v>45987</v>
       </c>
       <c r="B1393" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="C1393" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="D1393" t="s">
         <v>47</v>
@@ -41839,10 +41865,10 @@
         <v>45987</v>
       </c>
       <c r="B1394" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
       <c r="C1394" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="D1394" t="s">
         <v>21</v>
@@ -41862,10 +41888,10 @@
         <v>45987</v>
       </c>
       <c r="B1395" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="C1395" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="D1395" t="s">
         <v>26</v>
@@ -41885,10 +41911,10 @@
         <v>45987</v>
       </c>
       <c r="B1396" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="C1396" t="s">
-        <v>2862</v>
+        <v>2860</v>
       </c>
       <c r="D1396" t="s">
         <v>224</v>
@@ -41908,10 +41934,10 @@
         <v>45987</v>
       </c>
       <c r="B1397" t="s">
-        <v>2863</v>
+        <v>2861</v>
       </c>
       <c r="C1397" t="s">
-        <v>2864</v>
+        <v>2862</v>
       </c>
       <c r="D1397" t="s">
         <v>21</v>
@@ -41931,10 +41957,10 @@
         <v>45987</v>
       </c>
       <c r="B1398" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="C1398" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
       <c r="D1398" t="s">
         <v>224</v>
@@ -41954,10 +41980,10 @@
         <v>45987</v>
       </c>
       <c r="B1399" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
       <c r="C1399" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
       <c r="D1399" t="s">
         <v>26</v>
@@ -41977,13 +42003,13 @@
         <v>45987</v>
       </c>
       <c r="B1400" t="s">
+        <v>2868</v>
+      </c>
+      <c r="C1400" t="s">
+        <v>2869</v>
+      </c>
+      <c r="D1400" t="s">
         <v>2870</v>
-      </c>
-      <c r="C1400" t="s">
-        <v>2871</v>
-      </c>
-      <c r="D1400" t="s">
-        <v>2872</v>
       </c>
       <c r="E1400" t="s">
         <v>22</v>
@@ -42000,10 +42026,10 @@
         <v>45987</v>
       </c>
       <c r="B1401" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="C1401" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
       <c r="D1401" t="s">
         <v>50</v>
@@ -42023,10 +42049,10 @@
         <v>45987</v>
       </c>
       <c r="B1402" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
       <c r="C1402" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
       <c r="D1402" t="s">
         <v>155</v>
@@ -42035,7 +42061,7 @@
         <v>27</v>
       </c>
       <c r="F1402" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1402">
         <v>0</v>
@@ -42046,10 +42072,10 @@
         <v>45987</v>
       </c>
       <c r="B1403" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
       <c r="C1403" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
       <c r="D1403" t="s">
         <v>21</v>
@@ -42058,7 +42084,7 @@
         <v>94</v>
       </c>
       <c r="F1403" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1403">
         <v>0</v>
@@ -42069,10 +42095,10 @@
         <v>45987</v>
       </c>
       <c r="B1404" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="C1404" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="D1404" t="s">
         <v>39</v>
@@ -42081,7 +42107,7 @@
         <v>27</v>
       </c>
       <c r="F1404" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1404">
         <v>0</v>
@@ -42092,10 +42118,10 @@
         <v>45987</v>
       </c>
       <c r="B1405" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="C1405" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="D1405" t="s">
         <v>17</v>
@@ -42115,10 +42141,10 @@
         <v>45987</v>
       </c>
       <c r="B1406" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
       <c r="C1406" t="s">
-        <v>2884</v>
+        <v>2882</v>
       </c>
       <c r="D1406" t="s">
         <v>26</v>
@@ -42127,7 +42153,7 @@
         <v>27</v>
       </c>
       <c r="F1406" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1406">
         <v>0</v>
@@ -42138,10 +42164,10 @@
         <v>45987</v>
       </c>
       <c r="B1407" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
       <c r="C1407" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
       <c r="D1407" t="s">
         <v>8</v>
@@ -42161,10 +42187,10 @@
         <v>45987</v>
       </c>
       <c r="B1408" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="C1408" t="s">
-        <v>2888</v>
+        <v>2886</v>
       </c>
       <c r="D1408" t="s">
         <v>47</v>
@@ -42184,10 +42210,10 @@
         <v>45987</v>
       </c>
       <c r="B1409" t="s">
-        <v>2889</v>
+        <v>2887</v>
       </c>
       <c r="C1409" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
       <c r="D1409" t="s">
         <v>26</v>
@@ -42196,7 +42222,7 @@
         <v>27</v>
       </c>
       <c r="F1409" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G1409">
         <v>0</v>
@@ -42207,10 +42233,10 @@
         <v>45987</v>
       </c>
       <c r="B1410" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
       <c r="C1410" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
       <c r="D1410" t="s">
         <v>8</v>
@@ -42230,10 +42256,10 @@
         <v>45987</v>
       </c>
       <c r="B1411" t="s">
-        <v>2893</v>
+        <v>2891</v>
       </c>
       <c r="C1411" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
       <c r="D1411" t="s">
         <v>8</v>
@@ -42253,10 +42279,10 @@
         <v>45987</v>
       </c>
       <c r="B1412" t="s">
-        <v>2895</v>
+        <v>2893</v>
       </c>
       <c r="C1412" t="s">
-        <v>2896</v>
+        <v>2894</v>
       </c>
       <c r="D1412" t="s">
         <v>8</v>
@@ -42276,10 +42302,10 @@
         <v>45987</v>
       </c>
       <c r="B1413" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
       <c r="C1413" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
       <c r="D1413" t="s">
         <v>47</v>
@@ -42288,7 +42314,7 @@
         <v>9</v>
       </c>
       <c r="F1413" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1413">
         <v>0</v>
@@ -42299,10 +42325,10 @@
         <v>45987</v>
       </c>
       <c r="B1414" t="s">
-        <v>2899</v>
+        <v>2897</v>
       </c>
       <c r="C1414" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
       <c r="D1414" t="s">
         <v>50</v>
@@ -42322,10 +42348,10 @@
         <v>45987</v>
       </c>
       <c r="B1415" t="s">
-        <v>2901</v>
+        <v>2899</v>
       </c>
       <c r="C1415" t="s">
-        <v>2902</v>
+        <v>2900</v>
       </c>
       <c r="D1415" t="s">
         <v>31</v>
@@ -42345,10 +42371,10 @@
         <v>45987</v>
       </c>
       <c r="B1416" t="s">
-        <v>2903</v>
+        <v>2901</v>
       </c>
       <c r="C1416" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
       <c r="D1416" t="s">
         <v>8</v>
@@ -42368,10 +42394,10 @@
         <v>45987</v>
       </c>
       <c r="B1417" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="C1417" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="D1417" t="s">
         <v>17</v>
@@ -42391,10 +42417,10 @@
         <v>45987</v>
       </c>
       <c r="B1418" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
       <c r="C1418" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="D1418" t="s">
         <v>50</v>
@@ -42403,7 +42429,7 @@
         <v>27</v>
       </c>
       <c r="F1418" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1418">
         <v>0</v>
@@ -42414,10 +42440,10 @@
         <v>45987</v>
       </c>
       <c r="B1419" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="C1419" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
       <c r="D1419" t="s">
         <v>17</v>
@@ -42437,10 +42463,10 @@
         <v>45987</v>
       </c>
       <c r="B1420" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
       <c r="C1420" t="s">
-        <v>2912</v>
+        <v>2910</v>
       </c>
       <c r="D1420" t="s">
         <v>155</v>
@@ -42460,10 +42486,10 @@
         <v>45987</v>
       </c>
       <c r="B1421" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
       <c r="C1421" t="s">
-        <v>2914</v>
+        <v>2912</v>
       </c>
       <c r="D1421" t="s">
         <v>59</v>
@@ -42495,7 +42521,7 @@
         <v>9</v>
       </c>
       <c r="F1422" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1422">
         <v>0</v>
@@ -42506,10 +42532,10 @@
         <v>45987</v>
       </c>
       <c r="B1423" t="s">
-        <v>2915</v>
+        <v>2913</v>
       </c>
       <c r="C1423" t="s">
-        <v>2916</v>
+        <v>2914</v>
       </c>
       <c r="D1423" t="s">
         <v>21</v>
@@ -42529,10 +42555,10 @@
         <v>45987</v>
       </c>
       <c r="B1424" t="s">
-        <v>2917</v>
+        <v>2915</v>
       </c>
       <c r="C1424" t="s">
-        <v>2918</v>
+        <v>2916</v>
       </c>
       <c r="D1424" t="s">
         <v>17</v>
@@ -42541,7 +42567,7 @@
         <v>27</v>
       </c>
       <c r="F1424" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1424">
         <v>0</v>
@@ -42552,10 +42578,10 @@
         <v>45987</v>
       </c>
       <c r="B1425" t="s">
-        <v>2919</v>
+        <v>2917</v>
       </c>
       <c r="C1425" t="s">
-        <v>2920</v>
+        <v>2918</v>
       </c>
       <c r="D1425" t="s">
         <v>26</v>
@@ -42575,10 +42601,10 @@
         <v>45987</v>
       </c>
       <c r="B1426" t="s">
-        <v>2921</v>
+        <v>2919</v>
       </c>
       <c r="C1426" t="s">
-        <v>2922</v>
+        <v>2920</v>
       </c>
       <c r="D1426" t="s">
         <v>13</v>
@@ -42598,10 +42624,10 @@
         <v>45987</v>
       </c>
       <c r="B1427" t="s">
-        <v>2923</v>
+        <v>2921</v>
       </c>
       <c r="C1427" t="s">
-        <v>2924</v>
+        <v>2922</v>
       </c>
       <c r="D1427" t="s">
         <v>155</v>
@@ -42610,7 +42636,10 @@
         <v>9</v>
       </c>
       <c r="F1427" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="G1427">
+        <v>0</v>
       </c>
     </row>
     <row r="1428" spans="1:7" x14ac:dyDescent="0.25">
@@ -42618,10 +42647,10 @@
         <v>45987</v>
       </c>
       <c r="B1428" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
       <c r="C1428" t="s">
-        <v>2926</v>
+        <v>2924</v>
       </c>
       <c r="D1428" t="s">
         <v>8</v>
@@ -42641,10 +42670,10 @@
         <v>45987</v>
       </c>
       <c r="B1429" t="s">
-        <v>2927</v>
+        <v>2925</v>
       </c>
       <c r="C1429" t="s">
-        <v>2928</v>
+        <v>2926</v>
       </c>
       <c r="D1429" t="s">
         <v>17</v>
@@ -42664,10 +42693,10 @@
         <v>45987</v>
       </c>
       <c r="B1430" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
       <c r="C1430" t="s">
-        <v>2930</v>
+        <v>2928</v>
       </c>
       <c r="D1430" t="s">
         <v>155</v>
@@ -42676,7 +42705,7 @@
         <v>9</v>
       </c>
       <c r="F1430" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1430">
         <v>0</v>
@@ -42687,10 +42716,10 @@
         <v>45987</v>
       </c>
       <c r="B1431" t="s">
-        <v>2931</v>
+        <v>2929</v>
       </c>
       <c r="C1431" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
       <c r="D1431" t="s">
         <v>644</v>
@@ -42710,10 +42739,10 @@
         <v>45987</v>
       </c>
       <c r="B1432" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="C1432" t="s">
-        <v>2934</v>
+        <v>2932</v>
       </c>
       <c r="D1432" t="s">
         <v>17</v>
@@ -42722,7 +42751,7 @@
         <v>9</v>
       </c>
       <c r="F1432" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1432">
         <v>0</v>
@@ -42733,10 +42762,10 @@
         <v>45987</v>
       </c>
       <c r="B1433" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
       <c r="C1433" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
       <c r="D1433" t="s">
         <v>31</v>
@@ -42756,10 +42785,10 @@
         <v>45987</v>
       </c>
       <c r="B1434" t="s">
-        <v>2937</v>
+        <v>2935</v>
       </c>
       <c r="C1434" t="s">
-        <v>2938</v>
+        <v>2936</v>
       </c>
       <c r="D1434" t="s">
         <v>50</v>
@@ -42779,10 +42808,10 @@
         <v>45987</v>
       </c>
       <c r="B1435" t="s">
-        <v>2939</v>
+        <v>2937</v>
       </c>
       <c r="C1435" t="s">
-        <v>2940</v>
+        <v>2938</v>
       </c>
       <c r="D1435" t="s">
         <v>39</v>
@@ -42802,10 +42831,10 @@
         <v>45987</v>
       </c>
       <c r="B1436" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="C1436" t="s">
-        <v>2942</v>
+        <v>2940</v>
       </c>
       <c r="D1436" t="s">
         <v>44</v>
@@ -42825,10 +42854,10 @@
         <v>45987</v>
       </c>
       <c r="B1437" t="s">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="C1437" t="s">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="D1437" t="s">
         <v>31</v>
@@ -42848,10 +42877,10 @@
         <v>45987</v>
       </c>
       <c r="B1438" t="s">
-        <v>2945</v>
+        <v>2943</v>
       </c>
       <c r="C1438" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="D1438" t="s">
         <v>26</v>
@@ -42871,10 +42900,10 @@
         <v>45987</v>
       </c>
       <c r="B1439" t="s">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="C1439" t="s">
-        <v>2948</v>
+        <v>2946</v>
       </c>
       <c r="D1439" t="s">
         <v>34</v>
@@ -42917,10 +42946,10 @@
         <v>45987</v>
       </c>
       <c r="B1441" t="s">
-        <v>2949</v>
+        <v>2947</v>
       </c>
       <c r="C1441" t="s">
-        <v>2950</v>
+        <v>2948</v>
       </c>
       <c r="D1441" t="s">
         <v>50</v>
@@ -42940,10 +42969,10 @@
         <v>45987</v>
       </c>
       <c r="B1442" t="s">
-        <v>2951</v>
+        <v>2949</v>
       </c>
       <c r="C1442" t="s">
-        <v>2952</v>
+        <v>2950</v>
       </c>
       <c r="D1442" t="s">
         <v>116</v>
@@ -42963,10 +42992,10 @@
         <v>45987</v>
       </c>
       <c r="B1443" t="s">
-        <v>2953</v>
+        <v>2951</v>
       </c>
       <c r="C1443" t="s">
-        <v>2954</v>
+        <v>2952</v>
       </c>
       <c r="D1443" t="s">
         <v>13</v>
@@ -42986,10 +43015,10 @@
         <v>45987</v>
       </c>
       <c r="B1444" t="s">
-        <v>2955</v>
+        <v>2953</v>
       </c>
       <c r="C1444" t="s">
-        <v>2956</v>
+        <v>2954</v>
       </c>
       <c r="D1444" t="s">
         <v>21</v>
@@ -43009,10 +43038,10 @@
         <v>45987</v>
       </c>
       <c r="B1445" t="s">
-        <v>2957</v>
+        <v>2955</v>
       </c>
       <c r="C1445" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
       <c r="D1445" t="s">
         <v>31</v>
@@ -43032,10 +43061,10 @@
         <v>45987</v>
       </c>
       <c r="B1446" t="s">
-        <v>2959</v>
+        <v>2957</v>
       </c>
       <c r="C1446" t="s">
-        <v>2960</v>
+        <v>2958</v>
       </c>
       <c r="D1446" t="s">
         <v>8</v>
@@ -43055,10 +43084,10 @@
         <v>45987</v>
       </c>
       <c r="B1447" t="s">
-        <v>2961</v>
+        <v>2959</v>
       </c>
       <c r="C1447" t="s">
-        <v>2962</v>
+        <v>2960</v>
       </c>
       <c r="D1447" t="s">
         <v>26</v>
@@ -43078,10 +43107,10 @@
         <v>45987</v>
       </c>
       <c r="B1448" t="s">
-        <v>2963</v>
+        <v>2961</v>
       </c>
       <c r="C1448" t="s">
-        <v>2964</v>
+        <v>2962</v>
       </c>
       <c r="D1448" t="s">
         <v>26</v>
@@ -43101,10 +43130,10 @@
         <v>45987</v>
       </c>
       <c r="B1449" t="s">
-        <v>2965</v>
+        <v>2963</v>
       </c>
       <c r="C1449" t="s">
-        <v>2966</v>
+        <v>2964</v>
       </c>
       <c r="D1449" t="s">
         <v>39</v>
@@ -43124,10 +43153,10 @@
         <v>45987</v>
       </c>
       <c r="B1450" t="s">
-        <v>2967</v>
+        <v>2965</v>
       </c>
       <c r="C1450" t="s">
-        <v>2968</v>
+        <v>2966</v>
       </c>
       <c r="D1450" t="s">
         <v>50</v>
@@ -43147,10 +43176,10 @@
         <v>45987</v>
       </c>
       <c r="B1451" t="s">
-        <v>2969</v>
+        <v>2967</v>
       </c>
       <c r="C1451" t="s">
-        <v>2970</v>
+        <v>2968</v>
       </c>
       <c r="D1451" t="s">
         <v>47</v>
@@ -43170,10 +43199,10 @@
         <v>45987</v>
       </c>
       <c r="B1452" t="s">
-        <v>2971</v>
+        <v>2969</v>
       </c>
       <c r="C1452" t="s">
-        <v>2972</v>
+        <v>2970</v>
       </c>
       <c r="D1452" t="s">
         <v>31</v>
@@ -43193,10 +43222,10 @@
         <v>45987</v>
       </c>
       <c r="B1453" t="s">
-        <v>2973</v>
+        <v>2971</v>
       </c>
       <c r="C1453" t="s">
-        <v>2974</v>
+        <v>2972</v>
       </c>
       <c r="D1453" t="s">
         <v>26</v>
@@ -43216,10 +43245,10 @@
         <v>45987</v>
       </c>
       <c r="B1454" t="s">
-        <v>2975</v>
+        <v>2973</v>
       </c>
       <c r="C1454" t="s">
-        <v>2976</v>
+        <v>2974</v>
       </c>
       <c r="D1454" t="s">
         <v>34</v>
@@ -43239,10 +43268,10 @@
         <v>45987</v>
       </c>
       <c r="B1455" t="s">
-        <v>2977</v>
+        <v>2975</v>
       </c>
       <c r="C1455" t="s">
-        <v>2978</v>
+        <v>2976</v>
       </c>
       <c r="D1455" t="s">
         <v>644</v>
@@ -43262,10 +43291,10 @@
         <v>45987</v>
       </c>
       <c r="B1456" t="s">
-        <v>2979</v>
+        <v>2977</v>
       </c>
       <c r="C1456" t="s">
-        <v>2980</v>
+        <v>2978</v>
       </c>
       <c r="D1456" t="s">
         <v>8</v>
@@ -43275,6 +43304,9 @@
       </c>
       <c r="F1456" t="s">
         <v>28</v>
+      </c>
+      <c r="G1456">
+        <v>0</v>
       </c>
     </row>
     <row r="1457" spans="1:7" x14ac:dyDescent="0.25">
@@ -43282,10 +43314,10 @@
         <v>45987</v>
       </c>
       <c r="B1457" t="s">
-        <v>2981</v>
+        <v>2979</v>
       </c>
       <c r="C1457" t="s">
-        <v>2982</v>
+        <v>2980</v>
       </c>
       <c r="D1457" t="s">
         <v>13</v>
@@ -43305,10 +43337,10 @@
         <v>45987</v>
       </c>
       <c r="B1458" t="s">
-        <v>2983</v>
+        <v>2981</v>
       </c>
       <c r="C1458" t="s">
-        <v>2984</v>
+        <v>2982</v>
       </c>
       <c r="D1458" t="s">
         <v>424</v>
@@ -43328,10 +43360,10 @@
         <v>45987</v>
       </c>
       <c r="B1459" t="s">
-        <v>2985</v>
+        <v>2983</v>
       </c>
       <c r="C1459" t="s">
-        <v>2986</v>
+        <v>2984</v>
       </c>
       <c r="D1459" t="s">
         <v>424</v>
@@ -43351,10 +43383,10 @@
         <v>45987</v>
       </c>
       <c r="B1460" t="s">
-        <v>2987</v>
+        <v>2985</v>
       </c>
       <c r="C1460" t="s">
-        <v>2988</v>
+        <v>2986</v>
       </c>
       <c r="D1460" t="s">
         <v>424</v>
@@ -43374,10 +43406,10 @@
         <v>45987</v>
       </c>
       <c r="B1461" t="s">
-        <v>2989</v>
+        <v>2987</v>
       </c>
       <c r="C1461" t="s">
-        <v>2990</v>
+        <v>2988</v>
       </c>
       <c r="D1461" t="s">
         <v>424</v>
@@ -43397,10 +43429,10 @@
         <v>45987</v>
       </c>
       <c r="B1462" t="s">
-        <v>2991</v>
+        <v>2989</v>
       </c>
       <c r="C1462" t="s">
-        <v>2992</v>
+        <v>2990</v>
       </c>
       <c r="D1462" t="s">
         <v>424</v>
@@ -43420,10 +43452,10 @@
         <v>45988</v>
       </c>
       <c r="B1463" t="s">
-        <v>2993</v>
+        <v>2991</v>
       </c>
       <c r="C1463" t="s">
-        <v>2994</v>
+        <v>2992</v>
       </c>
       <c r="D1463" t="s">
         <v>21</v>
@@ -43443,10 +43475,10 @@
         <v>45988</v>
       </c>
       <c r="B1464" t="s">
-        <v>2995</v>
+        <v>2993</v>
       </c>
       <c r="C1464" t="s">
-        <v>2996</v>
+        <v>2994</v>
       </c>
       <c r="D1464" t="s">
         <v>17</v>
@@ -43466,10 +43498,10 @@
         <v>45988</v>
       </c>
       <c r="B1465" t="s">
-        <v>2997</v>
+        <v>2995</v>
       </c>
       <c r="C1465" t="s">
-        <v>2998</v>
+        <v>2996</v>
       </c>
       <c r="D1465" t="s">
         <v>224</v>
@@ -43489,10 +43521,10 @@
         <v>45988</v>
       </c>
       <c r="B1466" t="s">
-        <v>2999</v>
+        <v>2997</v>
       </c>
       <c r="C1466" t="s">
-        <v>3000</v>
+        <v>2998</v>
       </c>
       <c r="D1466" t="s">
         <v>8</v>
@@ -43512,10 +43544,10 @@
         <v>45988</v>
       </c>
       <c r="B1467" t="s">
-        <v>3001</v>
+        <v>2999</v>
       </c>
       <c r="C1467" t="s">
-        <v>3002</v>
+        <v>3000</v>
       </c>
       <c r="D1467" t="s">
         <v>21</v>
@@ -43535,10 +43567,10 @@
         <v>45988</v>
       </c>
       <c r="B1468" t="s">
-        <v>3003</v>
+        <v>3001</v>
       </c>
       <c r="C1468" t="s">
-        <v>3004</v>
+        <v>3002</v>
       </c>
       <c r="D1468" t="s">
         <v>74</v>
@@ -43558,10 +43590,10 @@
         <v>45988</v>
       </c>
       <c r="B1469" t="s">
-        <v>3005</v>
+        <v>3003</v>
       </c>
       <c r="C1469" t="s">
-        <v>3006</v>
+        <v>3004</v>
       </c>
       <c r="D1469" t="s">
         <v>8</v>
@@ -43581,10 +43613,10 @@
         <v>45988</v>
       </c>
       <c r="B1470" t="s">
-        <v>3007</v>
+        <v>3005</v>
       </c>
       <c r="C1470" t="s">
-        <v>3008</v>
+        <v>3006</v>
       </c>
       <c r="D1470" t="s">
         <v>13</v>
@@ -43604,10 +43636,10 @@
         <v>45988</v>
       </c>
       <c r="B1471" t="s">
-        <v>3009</v>
+        <v>3007</v>
       </c>
       <c r="C1471" t="s">
-        <v>3010</v>
+        <v>3008</v>
       </c>
       <c r="D1471" t="s">
         <v>74</v>
@@ -43627,10 +43659,10 @@
         <v>45988</v>
       </c>
       <c r="B1472" t="s">
-        <v>3011</v>
+        <v>3009</v>
       </c>
       <c r="C1472" t="s">
-        <v>3012</v>
+        <v>3010</v>
       </c>
       <c r="D1472" t="s">
         <v>26</v>
@@ -43645,15 +43677,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1473" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1473" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1473" s="1">
         <v>45988</v>
       </c>
       <c r="B1473" t="s">
-        <v>3015</v>
+        <v>3013</v>
       </c>
       <c r="C1473" t="s">
-        <v>3016</v>
+        <v>3014</v>
       </c>
       <c r="D1473" t="s">
         <v>26</v>
@@ -43662,18 +43694,21 @@
         <v>9</v>
       </c>
       <c r="F1473" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1474" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G1473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1474" s="1">
         <v>45988</v>
       </c>
       <c r="B1474" t="s">
-        <v>3017</v>
+        <v>3015</v>
       </c>
       <c r="C1474" t="s">
-        <v>3018</v>
+        <v>3016</v>
       </c>
       <c r="D1474" t="s">
         <v>74</v>
@@ -43684,16 +43719,19 @@
       <c r="F1474" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1475" s="1">
         <v>45988</v>
       </c>
       <c r="B1475" t="s">
-        <v>3019</v>
+        <v>3017</v>
       </c>
       <c r="C1475" t="s">
-        <v>3020</v>
+        <v>3018</v>
       </c>
       <c r="D1475" t="s">
         <v>8</v>
@@ -43702,18 +43740,21 @@
         <v>9</v>
       </c>
       <c r="F1475" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1476" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G1475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1476" s="1">
         <v>45988</v>
       </c>
       <c r="B1476" t="s">
-        <v>3021</v>
+        <v>3019</v>
       </c>
       <c r="C1476" t="s">
-        <v>3022</v>
+        <v>3020</v>
       </c>
       <c r="D1476" t="s">
         <v>26</v>
@@ -43724,16 +43765,19 @@
       <c r="F1476" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1477" s="1">
         <v>45988</v>
       </c>
       <c r="B1477" t="s">
-        <v>3023</v>
+        <v>3021</v>
       </c>
       <c r="C1477" t="s">
-        <v>3024</v>
+        <v>3022</v>
       </c>
       <c r="D1477" t="s">
         <v>21</v>
@@ -43744,16 +43788,19 @@
       <c r="F1477" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1477">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1478" s="1">
         <v>45988</v>
       </c>
       <c r="B1478" t="s">
-        <v>3025</v>
+        <v>3023</v>
       </c>
       <c r="C1478" t="s">
-        <v>3026</v>
+        <v>3024</v>
       </c>
       <c r="D1478" t="s">
         <v>31</v>
@@ -43764,16 +43811,19 @@
       <c r="F1478" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="1479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1478">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1479" s="1">
         <v>45988</v>
       </c>
       <c r="B1479" t="s">
-        <v>3027</v>
+        <v>3025</v>
       </c>
       <c r="C1479" t="s">
-        <v>3028</v>
+        <v>3026</v>
       </c>
       <c r="D1479" t="s">
         <v>8</v>
@@ -43784,16 +43834,19 @@
       <c r="F1479" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1479">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1480" s="1">
         <v>45988</v>
       </c>
       <c r="B1480" t="s">
-        <v>3029</v>
+        <v>3027</v>
       </c>
       <c r="C1480" t="s">
-        <v>3030</v>
+        <v>3028</v>
       </c>
       <c r="D1480" t="s">
         <v>44</v>
@@ -43804,16 +43857,19 @@
       <c r="F1480" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1480">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1481" s="1">
         <v>45988</v>
       </c>
       <c r="B1481" t="s">
-        <v>3031</v>
+        <v>3029</v>
       </c>
       <c r="C1481" t="s">
-        <v>3032</v>
+        <v>3030</v>
       </c>
       <c r="D1481" t="s">
         <v>21</v>
@@ -43822,18 +43878,21 @@
         <v>94</v>
       </c>
       <c r="F1481" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1482" spans="1:6" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+      <c r="G1481" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1482" s="1">
         <v>45988</v>
       </c>
       <c r="B1482" t="s">
-        <v>3033</v>
+        <v>3031</v>
       </c>
       <c r="C1482" t="s">
-        <v>3034</v>
+        <v>3032</v>
       </c>
       <c r="D1482" t="s">
         <v>26</v>
@@ -43844,16 +43903,19 @@
       <c r="F1482" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1482">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1483" s="1">
         <v>45988</v>
       </c>
       <c r="B1483" t="s">
-        <v>3035</v>
+        <v>3033</v>
       </c>
       <c r="C1483" t="s">
-        <v>3036</v>
+        <v>3034</v>
       </c>
       <c r="D1483" t="s">
         <v>74</v>
@@ -43864,16 +43926,19 @@
       <c r="F1483" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1484" s="1">
         <v>45988</v>
       </c>
       <c r="B1484" t="s">
-        <v>3037</v>
+        <v>3035</v>
       </c>
       <c r="C1484" t="s">
-        <v>3038</v>
+        <v>3036</v>
       </c>
       <c r="D1484" t="s">
         <v>31</v>
@@ -43882,18 +43947,21 @@
         <v>9</v>
       </c>
       <c r="F1484" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1485" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G1484">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1485" s="1">
         <v>45988</v>
       </c>
       <c r="B1485" t="s">
-        <v>3039</v>
+        <v>3037</v>
       </c>
       <c r="C1485" t="s">
-        <v>3040</v>
+        <v>3038</v>
       </c>
       <c r="D1485" t="s">
         <v>31</v>
@@ -43904,16 +43972,19 @@
       <c r="F1485" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1485">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1486" s="1">
         <v>45988</v>
       </c>
       <c r="B1486" t="s">
-        <v>3041</v>
+        <v>3039</v>
       </c>
       <c r="C1486" t="s">
-        <v>3042</v>
+        <v>3040</v>
       </c>
       <c r="D1486" t="s">
         <v>155</v>
@@ -43924,16 +43995,19 @@
       <c r="F1486" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1486">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1487" s="1">
         <v>45988</v>
       </c>
       <c r="B1487" t="s">
-        <v>3043</v>
+        <v>3041</v>
       </c>
       <c r="C1487" t="s">
-        <v>3044</v>
+        <v>3042</v>
       </c>
       <c r="D1487" t="s">
         <v>155</v>
@@ -43944,16 +44018,19 @@
       <c r="F1487" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1487">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1488" s="1">
         <v>45988</v>
       </c>
       <c r="B1488" t="s">
-        <v>3045</v>
+        <v>3043</v>
       </c>
       <c r="C1488" t="s">
-        <v>3046</v>
+        <v>3044</v>
       </c>
       <c r="D1488" t="s">
         <v>59</v>
@@ -43964,16 +44041,19 @@
       <c r="F1488" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1488">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1489" s="1">
         <v>45988</v>
       </c>
       <c r="B1489" t="s">
-        <v>3047</v>
+        <v>3045</v>
       </c>
       <c r="C1489" t="s">
-        <v>3048</v>
+        <v>3046</v>
       </c>
       <c r="D1489" t="s">
         <v>155</v>
@@ -43984,16 +44064,19 @@
       <c r="F1489" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1489">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1490" s="1">
         <v>45988</v>
       </c>
       <c r="B1490" t="s">
-        <v>3049</v>
+        <v>3047</v>
       </c>
       <c r="C1490" t="s">
-        <v>3050</v>
+        <v>3048</v>
       </c>
       <c r="D1490" t="s">
         <v>26</v>
@@ -44004,19 +44087,22 @@
       <c r="F1490" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1490">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1491" s="1">
         <v>45988</v>
       </c>
       <c r="B1491" t="s">
+        <v>3049</v>
+      </c>
+      <c r="C1491" t="s">
+        <v>3050</v>
+      </c>
+      <c r="D1491" t="s">
         <v>3051</v>
-      </c>
-      <c r="C1491" t="s">
-        <v>3052</v>
-      </c>
-      <c r="D1491" t="s">
-        <v>3053</v>
       </c>
       <c r="E1491" t="s">
         <v>94</v>
@@ -44024,16 +44110,19 @@
       <c r="F1491" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1491">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1492" s="1">
         <v>45988</v>
       </c>
       <c r="B1492" t="s">
-        <v>3054</v>
+        <v>3052</v>
       </c>
       <c r="C1492" t="s">
-        <v>3055</v>
+        <v>3053</v>
       </c>
       <c r="D1492" t="s">
         <v>31</v>
@@ -44044,19 +44133,22 @@
       <c r="F1492" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1492">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1493" s="1">
         <v>45988</v>
       </c>
       <c r="B1493" t="s">
-        <v>3056</v>
+        <v>3054</v>
       </c>
       <c r="C1493" t="s">
-        <v>3057</v>
+        <v>3055</v>
       </c>
       <c r="D1493" t="s">
-        <v>3053</v>
+        <v>3051</v>
       </c>
       <c r="E1493" t="s">
         <v>94</v>
@@ -44064,16 +44156,19 @@
       <c r="F1493" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1493">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1494" s="1">
         <v>45988</v>
       </c>
       <c r="B1494" t="s">
-        <v>3058</v>
+        <v>3056</v>
       </c>
       <c r="C1494" t="s">
-        <v>3059</v>
+        <v>3057</v>
       </c>
       <c r="D1494" t="s">
         <v>17</v>
@@ -44082,18 +44177,21 @@
         <v>9</v>
       </c>
       <c r="F1494" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1495" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G1494">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1495" s="1">
         <v>45988</v>
       </c>
       <c r="B1495" t="s">
-        <v>3060</v>
+        <v>3058</v>
       </c>
       <c r="C1495" t="s">
-        <v>3061</v>
+        <v>3059</v>
       </c>
       <c r="D1495" t="s">
         <v>17</v>
@@ -44104,16 +44202,19 @@
       <c r="F1495" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1495">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1496" s="1">
         <v>45988</v>
       </c>
       <c r="B1496" t="s">
-        <v>3062</v>
+        <v>3060</v>
       </c>
       <c r="C1496" t="s">
-        <v>3063</v>
+        <v>3061</v>
       </c>
       <c r="D1496" t="s">
         <v>74</v>
@@ -44124,16 +44225,19 @@
       <c r="F1496" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1496">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1497" s="1">
         <v>45988</v>
       </c>
       <c r="B1497" t="s">
-        <v>3064</v>
+        <v>3062</v>
       </c>
       <c r="C1497" t="s">
-        <v>3065</v>
+        <v>3063</v>
       </c>
       <c r="D1497" t="s">
         <v>21</v>
@@ -44144,16 +44248,19 @@
       <c r="F1497" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1497">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1498" s="1">
         <v>45988</v>
       </c>
       <c r="B1498" t="s">
-        <v>3066</v>
+        <v>3064</v>
       </c>
       <c r="C1498" t="s">
-        <v>3067</v>
+        <v>3065</v>
       </c>
       <c r="D1498" t="s">
         <v>44</v>
@@ -44164,16 +44271,19 @@
       <c r="F1498" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1498">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1499" s="1">
         <v>45988</v>
       </c>
       <c r="B1499" t="s">
-        <v>3068</v>
+        <v>3066</v>
       </c>
       <c r="C1499" t="s">
-        <v>3069</v>
+        <v>3067</v>
       </c>
       <c r="D1499" t="s">
         <v>34</v>
@@ -44184,16 +44294,19 @@
       <c r="F1499" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1499">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1500" s="1">
         <v>45988</v>
       </c>
       <c r="B1500" t="s">
-        <v>3070</v>
+        <v>3068</v>
       </c>
       <c r="C1500" t="s">
-        <v>3071</v>
+        <v>3069</v>
       </c>
       <c r="D1500" t="s">
         <v>26</v>
@@ -44204,16 +44317,19 @@
       <c r="F1500" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1501" s="1">
         <v>45988</v>
       </c>
       <c r="B1501" t="s">
-        <v>3072</v>
+        <v>3070</v>
       </c>
       <c r="C1501" t="s">
-        <v>3073</v>
+        <v>3071</v>
       </c>
       <c r="D1501" t="s">
         <v>17</v>
@@ -44224,16 +44340,19 @@
       <c r="F1501" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1501">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1502" s="1">
         <v>45988</v>
       </c>
       <c r="B1502" t="s">
-        <v>3074</v>
+        <v>3072</v>
       </c>
       <c r="C1502" t="s">
-        <v>3075</v>
+        <v>3073</v>
       </c>
       <c r="D1502" t="s">
         <v>17</v>
@@ -44244,16 +44363,19 @@
       <c r="F1502" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1502">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1503" s="1">
         <v>45988</v>
       </c>
       <c r="B1503" t="s">
-        <v>3076</v>
+        <v>3074</v>
       </c>
       <c r="C1503" t="s">
-        <v>3077</v>
+        <v>3075</v>
       </c>
       <c r="D1503" t="s">
         <v>8</v>
@@ -44264,16 +44386,19 @@
       <c r="F1503" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1503">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1504" s="1">
         <v>45988</v>
       </c>
       <c r="B1504" t="s">
-        <v>3078</v>
+        <v>3076</v>
       </c>
       <c r="C1504" t="s">
-        <v>3079</v>
+        <v>3077</v>
       </c>
       <c r="D1504" t="s">
         <v>8</v>
@@ -44284,16 +44409,19 @@
       <c r="F1504" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1504">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1505" s="1">
         <v>45988</v>
       </c>
       <c r="B1505" t="s">
-        <v>3080</v>
+        <v>3078</v>
       </c>
       <c r="C1505" t="s">
-        <v>3081</v>
+        <v>3079</v>
       </c>
       <c r="D1505" t="s">
         <v>31</v>
@@ -44304,16 +44432,19 @@
       <c r="F1505" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1505">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1506" s="1">
         <v>45988</v>
       </c>
       <c r="B1506" t="s">
-        <v>3082</v>
+        <v>3080</v>
       </c>
       <c r="C1506" t="s">
-        <v>3083</v>
+        <v>3081</v>
       </c>
       <c r="D1506" t="s">
         <v>50</v>
@@ -44324,16 +44455,19 @@
       <c r="F1506" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1506">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1507" s="1">
         <v>45988</v>
       </c>
       <c r="B1507" t="s">
-        <v>3084</v>
+        <v>3082</v>
       </c>
       <c r="C1507" t="s">
-        <v>3085</v>
+        <v>3083</v>
       </c>
       <c r="D1507" t="s">
         <v>74</v>
@@ -44342,18 +44476,21 @@
         <v>9</v>
       </c>
       <c r="F1507" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1508" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G1507">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1508" s="1">
         <v>45988</v>
       </c>
       <c r="B1508" t="s">
-        <v>3086</v>
+        <v>3084</v>
       </c>
       <c r="C1508" t="s">
-        <v>3087</v>
+        <v>3085</v>
       </c>
       <c r="D1508" t="s">
         <v>17</v>
@@ -44362,18 +44499,21 @@
         <v>9</v>
       </c>
       <c r="F1508" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1509" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G1508">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1509" s="1">
         <v>45988</v>
       </c>
       <c r="B1509" t="s">
-        <v>3088</v>
+        <v>3086</v>
       </c>
       <c r="C1509" t="s">
-        <v>3089</v>
+        <v>3087</v>
       </c>
       <c r="D1509" t="s">
         <v>644</v>
@@ -44384,16 +44524,19 @@
       <c r="F1509" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1509">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1510" s="1">
         <v>45988</v>
       </c>
       <c r="B1510" t="s">
-        <v>3090</v>
+        <v>3088</v>
       </c>
       <c r="C1510" t="s">
-        <v>3091</v>
+        <v>3089</v>
       </c>
       <c r="D1510" t="s">
         <v>116</v>
@@ -44404,16 +44547,19 @@
       <c r="F1510" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1510">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1511" s="1">
         <v>45988</v>
       </c>
       <c r="B1511" t="s">
-        <v>3092</v>
+        <v>3090</v>
       </c>
       <c r="C1511" t="s">
-        <v>3093</v>
+        <v>3091</v>
       </c>
       <c r="D1511" t="s">
         <v>34</v>
@@ -44424,16 +44570,19 @@
       <c r="F1511" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1511">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1512" s="1">
         <v>45988</v>
       </c>
       <c r="B1512" t="s">
-        <v>3094</v>
+        <v>3092</v>
       </c>
       <c r="C1512" t="s">
-        <v>3095</v>
+        <v>3093</v>
       </c>
       <c r="D1512" t="s">
         <v>59</v>
@@ -44444,16 +44593,19 @@
       <c r="F1512" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1512">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1513" s="1">
         <v>45988</v>
       </c>
       <c r="B1513" t="s">
-        <v>3096</v>
+        <v>3094</v>
       </c>
       <c r="C1513" t="s">
-        <v>3097</v>
+        <v>3095</v>
       </c>
       <c r="D1513" t="s">
         <v>17</v>
@@ -44464,16 +44616,19 @@
       <c r="F1513" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1513">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1514" s="1">
         <v>45988</v>
       </c>
       <c r="B1514" t="s">
-        <v>3098</v>
+        <v>3096</v>
       </c>
       <c r="C1514" t="s">
-        <v>3099</v>
+        <v>3097</v>
       </c>
       <c r="D1514" t="s">
         <v>17</v>
@@ -44484,16 +44639,19 @@
       <c r="F1514" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1514">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1515" s="1">
         <v>45988</v>
       </c>
       <c r="B1515" t="s">
-        <v>3100</v>
+        <v>3098</v>
       </c>
       <c r="C1515" t="s">
-        <v>3101</v>
+        <v>3099</v>
       </c>
       <c r="D1515" t="s">
         <v>44</v>
@@ -44502,18 +44660,21 @@
         <v>9</v>
       </c>
       <c r="F1515" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="1516" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G1515">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1516" s="1">
         <v>45988</v>
       </c>
       <c r="B1516" t="s">
-        <v>3102</v>
+        <v>3100</v>
       </c>
       <c r="C1516" t="s">
-        <v>3103</v>
+        <v>3101</v>
       </c>
       <c r="D1516" t="s">
         <v>59</v>
@@ -44524,16 +44685,19 @@
       <c r="F1516" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1516">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1517" s="1">
         <v>45988</v>
       </c>
       <c r="B1517" t="s">
-        <v>3104</v>
+        <v>3102</v>
       </c>
       <c r="C1517" t="s">
-        <v>3105</v>
+        <v>3103</v>
       </c>
       <c r="D1517" t="s">
         <v>1430</v>
@@ -44544,16 +44708,19 @@
       <c r="F1517" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1518" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1517">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1518" s="1">
         <v>45988</v>
       </c>
       <c r="B1518" t="s">
-        <v>3106</v>
+        <v>3104</v>
       </c>
       <c r="C1518" t="s">
-        <v>3107</v>
+        <v>3105</v>
       </c>
       <c r="D1518" t="s">
         <v>44</v>
@@ -44564,16 +44731,19 @@
       <c r="F1518" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1519" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1518">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1519" s="1">
         <v>45988</v>
       </c>
       <c r="B1519" t="s">
-        <v>3108</v>
+        <v>3106</v>
       </c>
       <c r="C1519" t="s">
-        <v>3109</v>
+        <v>3107</v>
       </c>
       <c r="D1519" t="s">
         <v>21</v>
@@ -44584,16 +44754,19 @@
       <c r="F1519" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1519">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1520" s="1">
         <v>45988</v>
       </c>
       <c r="B1520" t="s">
-        <v>3110</v>
+        <v>3108</v>
       </c>
       <c r="C1520" t="s">
-        <v>3111</v>
+        <v>3109</v>
       </c>
       <c r="D1520" t="s">
         <v>644</v>
@@ -44604,16 +44777,19 @@
       <c r="F1520" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1520">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1521" s="1">
         <v>45988</v>
       </c>
       <c r="B1521" t="s">
-        <v>3112</v>
+        <v>3110</v>
       </c>
       <c r="C1521" t="s">
-        <v>3113</v>
+        <v>3111</v>
       </c>
       <c r="D1521" t="s">
         <v>34</v>
@@ -44624,16 +44800,19 @@
       <c r="F1521" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1521">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1522" s="1">
         <v>45988</v>
       </c>
       <c r="B1522" t="s">
-        <v>3114</v>
+        <v>3112</v>
       </c>
       <c r="C1522" t="s">
-        <v>3115</v>
+        <v>3113</v>
       </c>
       <c r="D1522" t="s">
         <v>34</v>
@@ -44644,16 +44823,19 @@
       <c r="F1522" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1523" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1522">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1523" s="1">
         <v>45988</v>
       </c>
       <c r="B1523" t="s">
-        <v>3116</v>
+        <v>3114</v>
       </c>
       <c r="C1523" t="s">
-        <v>3117</v>
+        <v>3115</v>
       </c>
       <c r="D1523" t="s">
         <v>47</v>
@@ -44664,16 +44846,19 @@
       <c r="F1523" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1524" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1523">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1524" s="1">
         <v>45988</v>
       </c>
       <c r="B1524" t="s">
-        <v>3118</v>
+        <v>3116</v>
       </c>
       <c r="C1524" t="s">
-        <v>3119</v>
+        <v>3117</v>
       </c>
       <c r="D1524" t="s">
         <v>116</v>
@@ -44684,16 +44869,19 @@
       <c r="F1524" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1525" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1524">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1525" s="1">
         <v>45988</v>
       </c>
       <c r="B1525" t="s">
-        <v>3120</v>
+        <v>3118</v>
       </c>
       <c r="C1525" t="s">
-        <v>3121</v>
+        <v>3119</v>
       </c>
       <c r="D1525" t="s">
         <v>74</v>
@@ -44704,16 +44892,19 @@
       <c r="F1525" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1526" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1525">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1526" s="1">
         <v>45988</v>
       </c>
       <c r="B1526" t="s">
-        <v>3122</v>
+        <v>3120</v>
       </c>
       <c r="C1526" t="s">
-        <v>3123</v>
+        <v>3121</v>
       </c>
       <c r="D1526" t="s">
         <v>31</v>
@@ -44724,8 +44915,11 @@
       <c r="F1526" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1527" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1526">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1527" s="1">
         <v>45988</v>
       </c>
@@ -44744,16 +44938,19 @@
       <c r="F1527" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1528" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1527">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1528" s="1">
         <v>45988</v>
       </c>
       <c r="B1528" t="s">
-        <v>3124</v>
+        <v>3122</v>
       </c>
       <c r="C1528" t="s">
-        <v>3125</v>
+        <v>3123</v>
       </c>
       <c r="D1528" t="s">
         <v>74</v>
@@ -44764,16 +44961,19 @@
       <c r="F1528" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="1529" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1528">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1529" s="1">
         <v>45988</v>
       </c>
       <c r="B1529" t="s">
-        <v>3126</v>
+        <v>3124</v>
       </c>
       <c r="C1529" t="s">
-        <v>3127</v>
+        <v>3125</v>
       </c>
       <c r="D1529" t="s">
         <v>74</v>
@@ -44783,6 +44983,101 @@
       </c>
       <c r="F1529" t="s">
         <v>28</v>
+      </c>
+      <c r="G1529">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1530" s="1">
+        <v>45989</v>
+      </c>
+      <c r="B1530" t="s">
+        <v>3126</v>
+      </c>
+      <c r="C1530" t="s">
+        <v>3127</v>
+      </c>
+      <c r="D1530" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1530" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1530" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1530">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1531" s="1">
+        <v>45989</v>
+      </c>
+      <c r="B1531" t="s">
+        <v>3128</v>
+      </c>
+      <c r="C1531" t="s">
+        <v>3129</v>
+      </c>
+      <c r="D1531" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1531" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1531" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1531">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1532" s="1">
+        <v>45989</v>
+      </c>
+      <c r="B1532" t="s">
+        <v>3130</v>
+      </c>
+      <c r="C1532" t="s">
+        <v>3131</v>
+      </c>
+      <c r="D1532" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1532" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1532" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1532">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1533" s="1">
+        <v>45989</v>
+      </c>
+      <c r="B1533" t="s">
+        <v>3132</v>
+      </c>
+      <c r="C1533" t="s">
+        <v>3133</v>
+      </c>
+      <c r="D1533" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1533" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1533" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1533">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>